<commit_message>
working reports for all departments
</commit_message>
<xml_diff>
--- a/ge/ge_template.xlsx
+++ b/ge/ge_template.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoetucker/LBS/ge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB452F4C-E8DD-7545-BF2C-8C317134E89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6D849B-987B-8140-8326-9835E090D608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gifts" sheetId="4" r:id="rId1"/>
     <sheet name="Endowments" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Endowments!$A$4:$W$4</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Gifts!$A$4:$V$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Endowments!$A$4:$T$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Gifts!$A$4:$S$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
   <si>
     <t>Unit</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Operating Balance</t>
   </si>
   <si>
-    <t>Max MTF Transfer Amt</t>
-  </si>
-  <si>
     <t>Fund Purpose</t>
   </si>
   <si>
@@ -86,12 +83,6 @@
     <t>Home Unit/Dept</t>
   </si>
   <si>
-    <t>Total Balance</t>
-  </si>
-  <si>
-    <t>MTF Authority</t>
-  </si>
-  <si>
     <t>Fund Restriction</t>
   </si>
   <si>
@@ -113,18 +104,12 @@
     <t>YTD Expenditure</t>
   </si>
   <si>
-    <t>Max MTF Trf Amt</t>
-  </si>
-  <si>
     <t>MTF_Authority</t>
   </si>
   <si>
     <t>FundRestriction</t>
   </si>
   <si>
-    <t>LBS Notes</t>
-  </si>
-  <si>
     <t>as of 12/31/22</t>
   </si>
   <si>
@@ -135,6 +120,9 @@
   </si>
   <si>
     <t>ENDOWMENTS</t>
+  </si>
+  <si>
+    <t>AUL/UL</t>
   </si>
 </sst>
 </file>
@@ -200,7 +188,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -228,12 +216,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -395,31 +377,49 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="4" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="7" fillId="10" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="3" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="8" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="7" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="7" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -428,37 +428,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="3" fillId="5" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -749,41 +725,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A899E671-F9B4-4874-9DAE-2E98C9A550B1}">
-  <dimension ref="A1:BQ16"/>
+  <dimension ref="A1:BN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:R3"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="58.83203125" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
     <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" customWidth="1"/>
     <col min="9" max="9" width="8.1640625" customWidth="1"/>
     <col min="10" max="10" width="6.5" customWidth="1"/>
     <col min="11" max="11" width="9.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" style="12" customWidth="1"/>
-    <col min="13" max="13" width="21.1640625" style="12" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="16.5" style="12" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" style="12" customWidth="1"/>
-    <col min="17" max="17" width="16.33203125" style="12" customWidth="1"/>
-    <col min="18" max="18" width="13.83203125" customWidth="1"/>
-    <col min="19" max="19" width="37.5" customWidth="1"/>
-    <col min="20" max="20" width="24" customWidth="1"/>
-    <col min="21" max="21" width="11.5" customWidth="1"/>
-    <col min="22" max="22" width="26.5" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="16.5" style="10" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" customWidth="1"/>
+    <col min="17" max="17" width="44.6640625" customWidth="1"/>
+    <col min="18" max="18" width="31" customWidth="1"/>
+    <col min="19" max="19" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" ht="16" thickBot="1">
+    <row r="1" spans="1:66" ht="16" thickBot="1">
       <c r="A1" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -799,46 +772,43 @@
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
     </row>
-    <row r="2" spans="1:69" ht="32">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:66" ht="32">
+      <c r="A2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="21" t="s">
+      <c r="B2" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="22" t="s">
         <v>9</v>
       </c>
       <c r="L2" s="8" t="s">
@@ -853,62 +823,48 @@
       <c r="O2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="18" t="s">
+      <c r="R2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="S2" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="T2" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="U2" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="V2" s="27" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="3" spans="1:69" ht="16">
-      <c r="A3" s="26"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="28"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
+    <row r="3" spans="1:66">
+      <c r="A3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
     </row>
-    <row r="4" spans="1:69">
+    <row r="4" spans="1:66">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
@@ -917,16 +873,16 @@
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>7</v>
@@ -937,50 +893,39 @@
       <c r="K4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="R4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="11" t="s">
+      <c r="S4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="S4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="T4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="5" spans="1:69" s="3" customFormat="1">
+    <row r="5" spans="1:66" s="3" customFormat="1">
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5"/>
+      <c r="P5"/>
     </row>
-    <row r="16" spans="1:69" s="1" customFormat="1">
+    <row r="16" spans="1:66" s="1" customFormat="1">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -992,12 +937,319 @@
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+      <c r="AB16"/>
+      <c r="AC16"/>
+      <c r="AD16"/>
+      <c r="AE16"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
+      <c r="AI16"/>
+      <c r="AJ16"/>
+      <c r="AK16"/>
+      <c r="AL16"/>
+      <c r="AM16"/>
+      <c r="AN16"/>
+      <c r="AO16"/>
+      <c r="AP16"/>
+      <c r="AQ16"/>
+      <c r="AR16"/>
+      <c r="AS16"/>
+      <c r="AT16"/>
+      <c r="AU16"/>
+      <c r="AV16"/>
+      <c r="AW16"/>
+      <c r="AX16"/>
+      <c r="AY16"/>
+      <c r="AZ16"/>
+      <c r="BA16"/>
+      <c r="BB16"/>
+      <c r="BC16"/>
+      <c r="BD16"/>
+      <c r="BE16"/>
+      <c r="BF16"/>
+      <c r="BG16"/>
+      <c r="BH16"/>
+      <c r="BI16"/>
+      <c r="BJ16"/>
+      <c r="BK16"/>
+      <c r="BL16"/>
+      <c r="BM16"/>
+      <c r="BN16"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A4:S4" xr:uid="{9553CD2B-A0D1-4ECE-B5FB-0B62E2C4C91B}"/>
+  <mergeCells count="16">
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26CC7C7-56C8-9D44-8CF9-0C733EEB6A60}">
+  <dimension ref="A1:BO16"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="57" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" customWidth="1"/>
+    <col min="10" max="10" width="6.5" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" style="10" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="20.1640625" style="10" customWidth="1"/>
+    <col min="15" max="15" width="16.5" style="10" customWidth="1"/>
+    <col min="16" max="16" width="13.83203125" customWidth="1"/>
+    <col min="17" max="17" width="20.5" style="10" customWidth="1"/>
+    <col min="18" max="18" width="48.6640625" customWidth="1"/>
+    <col min="19" max="19" width="28.5" customWidth="1"/>
+    <col min="20" max="20" width="11.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:67" ht="16" thickBot="1">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+    </row>
+    <row r="2" spans="1:67" ht="32">
+      <c r="A2" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="R2" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="T2" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:67" ht="16">
+      <c r="A3" s="19"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="17"/>
+      <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
+    </row>
+    <row r="4" spans="1:67">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="S4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:67" s="3" customFormat="1">
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5"/>
+      <c r="Q5" s="10"/>
+    </row>
+    <row r="16" spans="1:67" s="1" customFormat="1">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16"/>
+      <c r="Q16" s="10"/>
       <c r="R16"/>
       <c r="S16"/>
       <c r="T16"/>
@@ -1048,367 +1300,14 @@
       <c r="BM16"/>
       <c r="BN16"/>
       <c r="BO16"/>
-      <c r="BP16"/>
-      <c r="BQ16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:V4" xr:uid="{9553CD2B-A0D1-4ECE-B5FB-0B62E2C4C91B}"/>
-  <mergeCells count="18">
+  <autoFilter ref="A4:T4" xr:uid="{9553CD2B-A0D1-4ECE-B5FB-0B62E2C4C91B}"/>
+  <mergeCells count="16">
+    <mergeCell ref="P2:P3"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
     <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="J2:J3"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26CC7C7-56C8-9D44-8CF9-0C733EEB6A60}">
-  <dimension ref="A1:BR16"/>
-  <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R27" sqref="R27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="30.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="36.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="12.83203125" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" customWidth="1"/>
-    <col min="10" max="10" width="6.5" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" style="12" customWidth="1"/>
-    <col min="13" max="13" width="21.1640625" style="12" customWidth="1"/>
-    <col min="14" max="14" width="20.1640625" style="12" customWidth="1"/>
-    <col min="15" max="15" width="16.5" style="12" customWidth="1"/>
-    <col min="16" max="16" width="16.6640625" style="12" customWidth="1"/>
-    <col min="17" max="17" width="16.33203125" style="12" customWidth="1"/>
-    <col min="18" max="18" width="13.83203125" customWidth="1"/>
-    <col min="19" max="19" width="20.5" style="12" customWidth="1"/>
-    <col min="20" max="20" width="37.5" customWidth="1"/>
-    <col min="21" max="21" width="24" customWidth="1"/>
-    <col min="22" max="22" width="11.5" customWidth="1"/>
-    <col min="23" max="23" width="26.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:70" ht="16" thickBot="1">
-      <c r="A1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-    </row>
-    <row r="2" spans="1:70" ht="32">
-      <c r="A2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="R2" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="S2" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="T2" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="U2" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="V2" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="W2" s="27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:70" ht="16">
-      <c r="A3" s="26"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
-    </row>
-    <row r="4" spans="1:70">
-      <c r="A4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="U4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="W4" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:70" s="3" customFormat="1">
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5"/>
-      <c r="S5" s="12"/>
-    </row>
-    <row r="16" spans="1:70" s="1" customFormat="1">
-      <c r="A16"/>
-      <c r="B16"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
-      <c r="G16"/>
-      <c r="H16"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16"/>
-      <c r="S16" s="12"/>
-      <c r="T16"/>
-      <c r="U16"/>
-      <c r="V16"/>
-      <c r="W16"/>
-      <c r="X16"/>
-      <c r="Y16"/>
-      <c r="Z16"/>
-      <c r="AA16"/>
-      <c r="AB16"/>
-      <c r="AC16"/>
-      <c r="AD16"/>
-      <c r="AE16"/>
-      <c r="AF16"/>
-      <c r="AG16"/>
-      <c r="AH16"/>
-      <c r="AI16"/>
-      <c r="AJ16"/>
-      <c r="AK16"/>
-      <c r="AL16"/>
-      <c r="AM16"/>
-      <c r="AN16"/>
-      <c r="AO16"/>
-      <c r="AP16"/>
-      <c r="AQ16"/>
-      <c r="AR16"/>
-      <c r="AS16"/>
-      <c r="AT16"/>
-      <c r="AU16"/>
-      <c r="AV16"/>
-      <c r="AW16"/>
-      <c r="AX16"/>
-      <c r="AY16"/>
-      <c r="AZ16"/>
-      <c r="BA16"/>
-      <c r="BB16"/>
-      <c r="BC16"/>
-      <c r="BD16"/>
-      <c r="BE16"/>
-      <c r="BF16"/>
-      <c r="BG16"/>
-      <c r="BH16"/>
-      <c r="BI16"/>
-      <c r="BJ16"/>
-      <c r="BK16"/>
-      <c r="BL16"/>
-      <c r="BM16"/>
-      <c r="BN16"/>
-      <c r="BO16"/>
-      <c r="BP16"/>
-      <c r="BQ16"/>
-      <c r="BR16"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A4:W4" xr:uid="{9553CD2B-A0D1-4ECE-B5FB-0B62E2C4C91B}"/>
-  <mergeCells count="18">
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="W2:W3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="L3:O3"/>
     <mergeCell ref="G2:G3"/>
@@ -1416,6 +1315,11 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add report output changes
</commit_message>
<xml_diff>
--- a/ge/ge_template.xlsx
+++ b/ge/ge_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoetucker/LBS/ge/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A6D849B-987B-8140-8326-9835E090D608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A73DE3-56E4-DE48-AC5A-7C7284D185CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="32">
   <si>
     <t>Unit</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>AUL/UL</t>
+  </si>
+  <si>
+    <t>LBS Notes</t>
   </si>
 </sst>
 </file>
@@ -727,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A899E671-F9B4-4874-9DAE-2E98C9A550B1}">
   <dimension ref="A1:BN16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -752,6 +755,7 @@
     <col min="17" max="17" width="44.6640625" customWidth="1"/>
     <col min="18" max="18" width="31" customWidth="1"/>
     <col min="19" max="19" width="11.5" customWidth="1"/>
+    <col min="20" max="20" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" ht="16" thickBot="1">
@@ -835,6 +839,9 @@
       <c r="S2" s="16" t="s">
         <v>18</v>
       </c>
+      <c r="T2" s="16" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:66">
       <c r="A3" s="19"/>
@@ -858,6 +865,7 @@
       <c r="Q3" s="17"/>
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
+      <c r="T3" s="17"/>
     </row>
     <row r="4" spans="1:66">
       <c r="A4" s="4" t="s">
@@ -916,6 +924,9 @@
       </c>
       <c r="S4" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="T4" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:66" s="3" customFormat="1">
@@ -994,8 +1005,8 @@
       <c r="BN16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:S4" xr:uid="{9553CD2B-A0D1-4ECE-B5FB-0B62E2C4C91B}"/>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="T2:T3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="R2:R3"/>
@@ -1022,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D26CC7C7-56C8-9D44-8CF9-0C733EEB6A60}">
   <dimension ref="A1:BO16"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2:U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -1048,6 +1059,7 @@
     <col min="18" max="18" width="48.6640625" customWidth="1"/>
     <col min="19" max="19" width="28.5" customWidth="1"/>
     <col min="20" max="20" width="11.5" customWidth="1"/>
+    <col min="21" max="21" width="36.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" ht="16" thickBot="1">
@@ -1135,6 +1147,9 @@
       <c r="T2" s="16" t="s">
         <v>18</v>
       </c>
+      <c r="U2" s="16" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:67" ht="16">
       <c r="A3" s="19"/>
@@ -1161,6 +1176,7 @@
       <c r="R3" s="17"/>
       <c r="S3" s="17"/>
       <c r="T3" s="17"/>
+      <c r="U3" s="17"/>
     </row>
     <row r="4" spans="1:67">
       <c r="A4" s="5" t="s">
@@ -1222,6 +1238,9 @@
       </c>
       <c r="T4" s="5" t="s">
         <v>18</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:67" s="3" customFormat="1">
@@ -1302,8 +1321,13 @@
       <c r="BO16"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:T4" xr:uid="{9553CD2B-A0D1-4ECE-B5FB-0B62E2C4C91B}"/>
-  <mergeCells count="16">
+  <mergeCells count="17">
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="P2:P3"/>
     <mergeCell ref="R2:R3"/>
     <mergeCell ref="S2:S3"/>
@@ -1315,11 +1339,6 @@
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="J2:J3"/>
     <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>